<commit_message>
updated screwsBOM with number references to drawings
</commit_message>
<xml_diff>
--- a/thermalpad_calculations.xlsx
+++ b/thermalpad_calculations.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zara\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zara\Documents\node-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -585,23 +585,23 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.7890625" customWidth="1"/>
-    <col min="2" max="2" width="23.89453125" customWidth="1"/>
-    <col min="3" max="3" width="10.5234375" customWidth="1"/>
-    <col min="4" max="4" width="9.89453125" customWidth="1"/>
+    <col min="1" max="1" width="39.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="9.15625" customWidth="1"/>
-    <col min="9" max="9" width="30.20703125" customWidth="1"/>
-    <col min="12" max="12" width="38.1015625" customWidth="1"/>
-    <col min="13" max="13" width="22.5234375" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" customWidth="1"/>
+    <col min="9" max="9" width="30.21875" customWidth="1"/>
+    <col min="12" max="12" width="38.109375" customWidth="1"/>
+    <col min="13" max="13" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
         <v>4</v>
       </c>
@@ -615,7 +615,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -635,7 +635,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -655,7 +655,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -675,7 +675,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -695,7 +695,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -717,12 +717,12 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -730,7 +730,7 @@
         <v>1.1579999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -738,7 +738,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -746,7 +746,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -754,7 +754,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -762,15 +762,15 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -778,7 +778,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -787,7 +787,7 @@
         <v>19.200000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -796,7 +796,7 @@
         <v>4.8000000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>

</xml_diff>